<commit_message>
feat(java project): added class files to demonstate class, object, constructor, this and static keywords
</commit_message>
<xml_diff>
--- a/syllabus/Java_DSA.xlsx
+++ b/syllabus/Java_DSA.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Schedule\Documents\TIME_DK\time_work\3_Colleges\SRET\curriculum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2_TIME_College\SRET\sret-java-bsc-26\syllabus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AAEF791-3629-41B2-AF1F-862FF4236DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="137">
   <si>
     <t>Topic</t>
   </si>
@@ -51,12 +50,6 @@
     <t>if/else, switch, loops (for, while, do-while)</t>
   </si>
   <si>
-    <t>LeetCode #1480</t>
-  </si>
-  <si>
-    <t>Functions</t>
-  </si>
-  <si>
     <t>Method creation, parameters, return types</t>
   </si>
   <si>
@@ -430,13 +423,25 @@
   </si>
   <si>
     <t>Session</t>
+  </si>
+  <si>
+    <t>Remark</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>LeetCode #1480, 2073</t>
+  </si>
+  <si>
+    <t>Methods</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -450,6 +455,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -486,7 +498,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -500,16 +512,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="10">
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
       <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -525,7 +566,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -541,27 +581,14 @@
       </border>
     </dxf>
     <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -577,13 +604,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{23D16A7D-F4A0-47C1-ACC0-A22C6F69DFC3}" name="Table1" displayName="Table1" ref="A1:D46" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1" headerRowBorderDxfId="6" tableBorderDxfId="7">
-  <autoFilter ref="A1:D46" xr:uid="{23D16A7D-F4A0-47C1-ACC0-A22C6F69DFC3}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{1B44F8A4-7C0C-4F99-A0BF-6E423963CCA2}" name="Session" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{682D418F-2A11-4F9F-8767-1ADBD15506D6}" name="Topic" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{C61FB87D-74F9-480B-B805-E72CE0A5BDA6}" name="Subtopics" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{3AE24401-42CA-4A7D-8E1A-2D4BE5D0F229}" name="LeetCode Problems" dataDxfId="3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E46" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5">
+  <autoFilter ref="A1:E46"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Session" dataDxfId="4"/>
+    <tableColumn id="2" name="Topic" dataDxfId="3"/>
+    <tableColumn id="3" name="Subtopics" dataDxfId="2"/>
+    <tableColumn id="4" name="LeetCode Problems" dataDxfId="1"/>
+    <tableColumn id="5" name="Remark" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -851,24 +879,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -879,8 +908,11 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -893,8 +925,11 @@
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -905,612 +940,665 @@
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E41" s="2"/>
+    </row>
+    <row r="42" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E42" s="2"/>
+    </row>
+    <row r="43" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E43" s="2"/>
+    </row>
+    <row r="44" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="E44" s="2"/>
+    </row>
+    <row r="45" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E45" s="2"/>
+    </row>
+    <row r="46" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="E46" s="2"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+      <formula>$E$2</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>